<commit_message>
Update test files for FASTQ new naming requirement
</commit_message>
<xml_diff>
--- a/submit_cgap/tests/data/cgap_submit_simple.xlsx
+++ b/submit_cgap/tests/data/cgap_submit_simple.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kentpitman/py/SubmitCGAP/submit_cgap/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/SubmitCGAP/submit_cgap/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E090A731-19CC-B148-A846-BDB90B7A732D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6979EA-4801-D849-8740-79544C2A4475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="1780" windowWidth="28800" windowHeight="16460" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
+    <workbookView xWindow="0" yWindow="1540" windowWidth="28800" windowHeight="16460" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,13 +66,13 @@
     <t>Files</t>
   </si>
   <si>
-    <t>test1.fastq.gz, test2.fastq.gz</t>
-  </si>
-  <si>
     <t>indiv1</t>
   </si>
   <si>
     <t>Report Required*</t>
+  </si>
+  <si>
+    <t>test1_R1.fastq.gz, test1_R2.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -551,10 +551,10 @@
   <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -584,7 +584,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>7</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="2" spans="1:47" ht="15">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -665,7 +665,7 @@
         <v>4</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M2" s="5"/>
     </row>

</xml_diff>

<commit_message>
Merge recent master, bringing files up-to-date for changes from dcicutils 3.11.0 to 6.2.0, accepting the new env_utils, which would err if we used it, and making sure not to use it.
</commit_message>
<xml_diff>
--- a/submit_cgap/tests/data/cgap_submit_simple.xlsx
+++ b/submit_cgap/tests/data/cgap_submit_simple.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kentpitman/py/SubmitCGAP/submit_cgap/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/SubmitCGAP/submit_cgap/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E090A731-19CC-B148-A846-BDB90B7A732D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6979EA-4801-D849-8740-79544C2A4475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="1780" windowWidth="28800" windowHeight="16460" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
+    <workbookView xWindow="0" yWindow="1540" windowWidth="28800" windowHeight="16460" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,13 +66,13 @@
     <t>Files</t>
   </si>
   <si>
-    <t>test1.fastq.gz, test2.fastq.gz</t>
-  </si>
-  <si>
     <t>indiv1</t>
   </si>
   <si>
     <t>Report Required*</t>
+  </si>
+  <si>
+    <t>test1_R1.fastq.gz, test1_R2.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -551,10 +551,10 @@
   <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -584,7 +584,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>7</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="2" spans="1:47" ht="15">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -665,7 +665,7 @@
         <v>4</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M2" s="5"/>
     </row>

</xml_diff>